<commit_message>
minor: remove blank sheets
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/merge.xlsx
+++ b/src/main/webapp/WEB-INF/books/merge.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="17040" windowHeight="11280"/>
+    <workbookView xWindow="360" yWindow="340" windowWidth="17040" windowHeight="11280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -29,8 +33,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,14 +376,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -438,24 +442,11 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B2:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>